<commit_message>
made a bit of update
</commit_message>
<xml_diff>
--- a/Group26Status.xlsx
+++ b/Group26Status.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentutsedu-my.sharepoint.com/personal/jungwook_van-1_student_uts_edu_au/Documents/UTS2025/31264 32501 Computer Graphics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="201" documentId="11_F25DC773A252ABDACC1048F9E99F732C5ADE58E4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02031B54-9395-4BE5-A8F2-7F9DEFA226DF}"/>
+  <xr:revisionPtr revIDLastSave="327" documentId="11_F25DC773A252ABDACC1048F9E99F732C5ADE58E4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{817128B4-C933-4105-833A-C2C5FC4D243E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignemnt3.1" sheetId="1" r:id="rId1"/>
     <sheet name="Assignment3.2" sheetId="2" r:id="rId2"/>
     <sheet name="Assignment3.3 Individual " sheetId="3" r:id="rId3"/>
     <sheet name="Assignment Group Projects" sheetId="5" r:id="rId4"/>
-    <sheet name="Gantt Chart" sheetId="6" r:id="rId5"/>
-    <sheet name="Git-Branching Guidance" sheetId="4" r:id="rId6"/>
+    <sheet name="Git-Branching Guidance" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="263">
   <si>
     <t>RAG Project Status</t>
   </si>
@@ -449,13 +448,592 @@
   </si>
   <si>
     <t>Git-Branching Guidance'!A1</t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>1. Project Setup</t>
+  </si>
+  <si>
+    <t>Create GitHub repository and structure</t>
+  </si>
+  <si>
+    <t>Install dependencies and configure tools</t>
+  </si>
+  <si>
+    <t>Set up basic Three.js scene</t>
+  </si>
+  <si>
+    <t>2. Planning</t>
+  </si>
+  <si>
+    <t>Define project scope and functionality</t>
+  </si>
+  <si>
+    <t>Break down tasks and assign responsibilities</t>
+  </si>
+  <si>
+    <t>3. Modeling</t>
+  </si>
+  <si>
+    <t>Design and create 3D models (e.g., objects, environment)</t>
+  </si>
+  <si>
+    <t>Apply textures and optimize models</t>
+  </si>
+  <si>
+    <t>4. Core Features</t>
+  </si>
+  <si>
+    <t>Implement camera controls</t>
+  </si>
+  <si>
+    <t>Add lighting (ambient, directional)</t>
+  </si>
+  <si>
+    <t>Enable object placement and interaction</t>
+  </si>
+  <si>
+    <t>5. Integration</t>
+  </si>
+  <si>
+    <t>Integrate models into the scene</t>
+  </si>
+  <si>
+    <t>Add UI elements (buttons, menus)</t>
+  </si>
+  <si>
+    <t>6. Testing &amp; Debugging</t>
+  </si>
+  <si>
+    <t>Test functionality and fix bugs</t>
+  </si>
+  <si>
+    <t>Optimize performance</t>
+  </si>
+  <si>
+    <t>7. Deployment</t>
+  </si>
+  <si>
+    <t>Prepare final build</t>
+  </si>
+  <si>
+    <t>Deploy to GitHub Pages</t>
+  </si>
+  <si>
+    <t>Task Status</t>
+  </si>
+  <si>
+    <t>날짜</t>
+  </si>
+  <si>
+    <t>작업 내용</t>
+  </si>
+  <si>
+    <t>비고</t>
+  </si>
+  <si>
+    <t>1일차 (D-14)</t>
+  </si>
+  <si>
+    <t>- 프로젝트 기획</t>
+  </si>
+  <si>
+    <t>- 핵심 기능 정의</t>
+  </si>
+  <si>
+    <t>- 개발환경 세팅 (Three.js 등)</t>
+  </si>
+  <si>
+    <t>시작 준비 단계</t>
+  </si>
+  <si>
+    <t>2일차 (D-13)</t>
+  </si>
+  <si>
+    <t>- 기본 지형 생성</t>
+  </si>
+  <si>
+    <t>- 카메라 및 조작 컨트롤 구현 (OrbitControls 등)</t>
+  </si>
+  <si>
+    <t>지형 렌더링 확인</t>
+  </si>
+  <si>
+    <t>3일차 (D-12)</t>
+  </si>
+  <si>
+    <t>- 구조물 오브젝트 임포트/모델링 (간단한 Cube로 시작 가능)</t>
+  </si>
+  <si>
+    <t>4일차 (D-11)</t>
+  </si>
+  <si>
+    <t>- 구조물 배치 시스템 구현 (클릭으로 배치 등)</t>
+  </si>
+  <si>
+    <t>UI 없이 기능 위주 구현</t>
+  </si>
+  <si>
+    <t>5일차 (D-10)</t>
+  </si>
+  <si>
+    <t>- 오브젝트 간 충돌 감지 로직 구현</t>
+  </si>
+  <si>
+    <t>겹치기 방지</t>
+  </si>
+  <si>
+    <t>6일차 (D-9)</t>
+  </si>
+  <si>
+    <t>- UI 요소 제작 시작 (버튼, 선택창 등)</t>
+  </si>
+  <si>
+    <t>- 기본 HUD 구성</t>
+  </si>
+  <si>
+    <t>7일차 (D-8)</t>
+  </si>
+  <si>
+    <t>- 동적 라이팅, 그림자 처리</t>
+  </si>
+  <si>
+    <t>- 낮/밤 라이트 테스트</t>
+  </si>
+  <si>
+    <t>Three.js 기본 조명 활용</t>
+  </si>
+  <si>
+    <t>8일차 (D-7)</t>
+  </si>
+  <si>
+    <t>- 지형 다양화 (언덕, 평지 등)</t>
+  </si>
+  <si>
+    <t>- 간단한 노이즈 지형 생성</t>
+  </si>
+  <si>
+    <t>선택 사항 (시간 여유 시)</t>
+  </si>
+  <si>
+    <t>9일차 (D-6)</t>
+  </si>
+  <si>
+    <t>- 자원 시스템 구현 (건물 배치 시 자원 소모 등)</t>
+  </si>
+  <si>
+    <t>미니멀 로직 구현</t>
+  </si>
+  <si>
+    <t>10일차 (D-5)</t>
+  </si>
+  <si>
+    <t>- UI 개선</t>
+  </si>
+  <si>
+    <t>- 구조물 선택 및 삭제 기능 추가</t>
+  </si>
+  <si>
+    <t>UX 향상</t>
+  </si>
+  <si>
+    <t>11일차 (D-4)</t>
+  </si>
+  <si>
+    <t>- 최적화 (렌더링, 메모리 관리 등)</t>
+  </si>
+  <si>
+    <t>- 코드 리팩토링</t>
+  </si>
+  <si>
+    <t>성능 개선 단계</t>
+  </si>
+  <si>
+    <t>12일차 (D-3)</t>
+  </si>
+  <si>
+    <t>- 테스트 및 디버깅</t>
+  </si>
+  <si>
+    <t>- 버그 수정</t>
+  </si>
+  <si>
+    <t>직접 플레이 테스트</t>
+  </si>
+  <si>
+    <t>13일차 (D-2)</t>
+  </si>
+  <si>
+    <t>- 최종 점검</t>
+  </si>
+  <si>
+    <t>- 사용자 흐름 테스트</t>
+  </si>
+  <si>
+    <t>피드백 받을 수 있으면 좋아요</t>
+  </si>
+  <si>
+    <t>14일차 (D-1)</t>
+  </si>
+  <si>
+    <t>- 배포 준비 (GitHub Pages 등)</t>
+  </si>
+  <si>
+    <t>- 결과 정리 (시연 영상 등)</t>
+  </si>
+  <si>
+    <t>포트폴리오용 정리</t>
+  </si>
+  <si>
+    <t>3D 생존 기지 건설 시뮬레이터</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <r>
+      <t>Main Branch (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>main</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Holds stable, deployable code with completed features ready for production.</t>
+  </si>
+  <si>
+    <r>
+      <t>Development Branch (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>dev</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>The central branch for ongoing work. Team members merge feature branches here after review.</t>
+  </si>
+  <si>
+    <t>Feature Branches</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Individual branches for specific tasks, e.g., </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>feature/terrain-generation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>feature/camera-controls</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Pull Requests (PR)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Merging feature branches into </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>dev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> via PRs for code review and team discussion.</t>
+    </r>
+  </si>
+  <si>
+    <t>Conflict Management</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Regularly pull from </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>dev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> into feature branches to update and resolve conflicts early.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Features are tested in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>dev</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> before merging into </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>main</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to ensure stability and functionality.</t>
+    </r>
+  </si>
+  <si>
+    <t>Issue Tracking</t>
+  </si>
+  <si>
+    <t>Use GitHub Issues to track tasks, bugs, and discussions for better team collaboration.</t>
+  </si>
+  <si>
+    <t>Demo Deployment</t>
+  </si>
+  <si>
+    <t>Deploy project previews via GitHub Pages for live demonstrations of progress.</t>
+  </si>
+  <si>
+    <t>Branch Name</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>Holds stable, deployable code for the interactive farm project.</t>
+  </si>
+  <si>
+    <t>dev</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The central integration branch where all features are merged for testing before finalizing in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>main</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>feature/terrain-system</t>
+  </si>
+  <si>
+    <t>Handles terrain generation (grass, soil, elevation) for a realistic farm environment.</t>
+  </si>
+  <si>
+    <t>feature/farm-objects</t>
+  </si>
+  <si>
+    <t>Adds interactive farm objects like barns, houses, fences, and other visuals.</t>
+  </si>
+  <si>
+    <t>feature/plant-system</t>
+  </si>
+  <si>
+    <t>Implements planting, growing, and harvesting of crops.</t>
+  </si>
+  <si>
+    <t>feature/animal-system</t>
+  </si>
+  <si>
+    <t>Manages animal interactions, including movement, behaviors, and sounds.</t>
+  </si>
+  <si>
+    <t>feature/user-controls</t>
+  </si>
+  <si>
+    <t>Develops user interaction, like camera movement, clicking, dragging, or hovering over objects.</t>
+  </si>
+  <si>
+    <t>feature/ui-elements</t>
+  </si>
+  <si>
+    <t>Implements UI components like menus, inventory systems, and notifications.</t>
+  </si>
+  <si>
+    <t>feature/environmental-effects</t>
+  </si>
+  <si>
+    <t>Adds weather effects (rain, sunlight, wind) to enhance the farm environment.</t>
+  </si>
+  <si>
+    <t>feature/sound-system</t>
+  </si>
+  <si>
+    <t>Integrates sound effects for animals, tools, and environmental sounds like rain or wind.</t>
+  </si>
+  <si>
+    <t>feature/multiplayer</t>
+  </si>
+  <si>
+    <t>(Optional) Implements multiplayer functionality for collaborative farm management.</t>
+  </si>
+  <si>
+    <t>feature/deploy-system</t>
+  </si>
+  <si>
+    <t>Prepares deployment scripts for hosting the farm project on platforms like GitHub Pages.</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -502,8 +1080,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.6"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -531,6 +1136,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -583,7 +1212,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -636,6 +1265,40 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1482,16 +2145,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CF0B44-1FED-4129-916C-F80D8E92DAC2}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="37.88671875" customWidth="1"/>
-    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.77734375" customWidth="1"/>
     <col min="3" max="3" width="46" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" customWidth="1"/>
@@ -1527,7 +2190,7 @@
       <c r="D2" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E2" s="9"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
@@ -1642,7 +2305,334 @@
         <v>99</v>
       </c>
     </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="29" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="28" t="s">
+        <v>167</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="10"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="28"/>
+      <c r="B18" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="10"/>
+    </row>
+    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="28"/>
+      <c r="B19" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="28"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="28"/>
+      <c r="B21" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="9"/>
+    </row>
+    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="9"/>
+    </row>
+    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C25" s="28"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="9"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="28"/>
+      <c r="B26" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C26" s="28"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="9"/>
+    </row>
+    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="9"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="28"/>
+      <c r="B28" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C28" s="28"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="9"/>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A29" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="9"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="28"/>
+      <c r="B30" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C30" s="28"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="9"/>
+    </row>
+    <row r="31" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="9"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C32" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="9"/>
+    </row>
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="28"/>
+      <c r="B33" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C33" s="28"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="9"/>
+    </row>
+    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>205</v>
+      </c>
+      <c r="D34" s="6"/>
+      <c r="E34" s="9"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="28"/>
+      <c r="B35" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="C35" s="28"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="9"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="28" t="s">
+        <v>206</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="C36" s="28" t="s">
+        <v>209</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="9"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="28"/>
+      <c r="B37" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C37" s="28"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="9"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="9"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="28"/>
+      <c r="B39" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C39" s="28"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="9"/>
+    </row>
+    <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="9"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="28"/>
+      <c r="B41" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="C41" s="28"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="9"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D43" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="20">
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="C25:C26"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1650,10 +2640,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D0A090-A0FD-4C12-8A63-D35993E32FAB}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1663,6 +2653,7 @@
     <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="45.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1835,7 +2826,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>132</v>
       </c>
@@ -1843,13 +2834,303 @@
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
         <v>133</v>
       </c>
       <c r="B18" s="23" t="s">
         <v>135</v>
       </c>
+    </row>
+    <row r="21" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="C22" s="26">
+        <v>45744</v>
+      </c>
+      <c r="D22" s="26">
+        <v>45745</v>
+      </c>
+      <c r="E22" s="25">
+        <v>2</v>
+      </c>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="25"/>
+      <c r="B23" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="26">
+        <v>45744</v>
+      </c>
+      <c r="D23" s="26">
+        <v>45745</v>
+      </c>
+      <c r="E23" s="25">
+        <v>2</v>
+      </c>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="25"/>
+      <c r="B24" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="26">
+        <v>45746</v>
+      </c>
+      <c r="D24" s="26">
+        <v>45747</v>
+      </c>
+      <c r="E24" s="25">
+        <v>2</v>
+      </c>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="C25" s="26">
+        <v>45748</v>
+      </c>
+      <c r="D25" s="26">
+        <v>45749</v>
+      </c>
+      <c r="E25" s="25">
+        <v>2</v>
+      </c>
+      <c r="F25" s="10"/>
+    </row>
+    <row r="26" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
+      <c r="B26" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" s="26">
+        <v>45748</v>
+      </c>
+      <c r="D26" s="26">
+        <v>45749</v>
+      </c>
+      <c r="E26" s="25">
+        <v>2</v>
+      </c>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="C27" s="26">
+        <v>45750</v>
+      </c>
+      <c r="D27" s="26">
+        <v>45757</v>
+      </c>
+      <c r="E27" s="25">
+        <v>8</v>
+      </c>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="25"/>
+      <c r="B28" s="25" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="26">
+        <v>45758</v>
+      </c>
+      <c r="D28" s="26">
+        <v>45760</v>
+      </c>
+      <c r="E28" s="25">
+        <v>3</v>
+      </c>
+      <c r="F28" s="9"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="26">
+        <v>45761</v>
+      </c>
+      <c r="D29" s="26">
+        <v>45762</v>
+      </c>
+      <c r="E29" s="25">
+        <v>2</v>
+      </c>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="25"/>
+      <c r="B30" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="C30" s="26">
+        <v>45763</v>
+      </c>
+      <c r="D30" s="26">
+        <v>45764</v>
+      </c>
+      <c r="E30" s="25">
+        <v>2</v>
+      </c>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="25"/>
+      <c r="B31" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="C31" s="26">
+        <v>45765</v>
+      </c>
+      <c r="D31" s="26">
+        <v>45768</v>
+      </c>
+      <c r="E31" s="25">
+        <v>4</v>
+      </c>
+      <c r="F31" s="9"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="24" t="s">
+        <v>154</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="C32" s="26">
+        <v>45769</v>
+      </c>
+      <c r="D32" s="26">
+        <v>45771</v>
+      </c>
+      <c r="E32" s="25">
+        <v>3</v>
+      </c>
+      <c r="F32" s="9"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="25"/>
+      <c r="B33" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C33" s="26">
+        <v>45772</v>
+      </c>
+      <c r="D33" s="26">
+        <v>45774</v>
+      </c>
+      <c r="E33" s="25">
+        <v>3</v>
+      </c>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" s="26">
+        <v>45775</v>
+      </c>
+      <c r="D34" s="26">
+        <v>45779</v>
+      </c>
+      <c r="E34" s="25">
+        <v>5</v>
+      </c>
+      <c r="F34" s="9"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="25"/>
+      <c r="B35" s="25" t="s">
+        <v>159</v>
+      </c>
+      <c r="C35" s="26">
+        <v>45780</v>
+      </c>
+      <c r="D35" s="26">
+        <v>45782</v>
+      </c>
+      <c r="E35" s="25">
+        <v>3</v>
+      </c>
+      <c r="F35" s="9"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" s="26">
+        <v>45783</v>
+      </c>
+      <c r="D36" s="26">
+        <v>45784</v>
+      </c>
+      <c r="E36" s="25">
+        <v>2</v>
+      </c>
+      <c r="F36" s="9"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="25"/>
+      <c r="B37" s="25" t="s">
+        <v>162</v>
+      </c>
+      <c r="C37" s="26">
+        <v>45785</v>
+      </c>
+      <c r="D37" s="26">
+        <v>45785</v>
+      </c>
+      <c r="E37" s="25">
+        <v>1</v>
+      </c>
+      <c r="F37" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1862,25 +3143,197 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1B36320-9BB1-4853-AB89-CD4A89CE0E11}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DC0284-78FD-4D6B-AB7A-95EC7E11330B}">
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DC0284-78FD-4D6B-AB7A-95EC7E11330B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="67.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>219</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>235</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>236</v>
+      </c>
+      <c r="F1" s="34" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>237</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="F2" s="35"/>
+    </row>
+    <row r="3" spans="1:6" ht="29.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
+        <v>222</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>239</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="F3" s="35"/>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
+        <v>224</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="F4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>243</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="F5" s="35"/>
+    </row>
+    <row r="6" spans="1:6" ht="29.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="14" t="s">
+        <v>228</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>245</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>246</v>
+      </c>
+      <c r="F6" s="36"/>
+    </row>
+    <row r="7" spans="1:6" ht="29.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>247</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>248</v>
+      </c>
+      <c r="F7" s="35"/>
+    </row>
+    <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="14" t="s">
+        <v>231</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>249</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>250</v>
+      </c>
+      <c r="F8" s="35"/>
+    </row>
+    <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>251</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="F9" s="36"/>
+    </row>
+    <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D10" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="F10" s="37"/>
+    </row>
+    <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D11" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>256</v>
+      </c>
+      <c r="F11" s="37"/>
+    </row>
+    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D12" s="32" t="s">
+        <v>257</v>
+      </c>
+      <c r="E12" s="33" t="s">
+        <v>258</v>
+      </c>
+      <c r="F12" s="37"/>
+    </row>
+    <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D13" s="32" t="s">
+        <v>259</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>260</v>
+      </c>
+      <c r="F13" s="37"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
made a slight changes
</commit_message>
<xml_diff>
--- a/Group26Status.xlsx
+++ b/Group26Status.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentutsedu-my.sharepoint.com/personal/jungwook_van-1_student_uts_edu_au/Documents/UTS2025/31264 32501 Computer Graphics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="327" documentId="11_F25DC773A252ABDACC1048F9E99F732C5ADE58E4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{817128B4-C933-4105-833A-C2C5FC4D243E}"/>
+  <xr:revisionPtr revIDLastSave="328" documentId="11_F25DC773A252ABDACC1048F9E99F732C5ADE58E4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A068F434-9786-4A2C-A604-E50EFC636640}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignemnt3.1" sheetId="1" r:id="rId1"/>
@@ -1277,10 +1277,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1299,6 +1296,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2147,7 +2147,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CF0B44-1FED-4129-916C-F80D8E92DAC2}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2306,7 +2306,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="28" t="s">
         <v>218</v>
       </c>
     </row>
@@ -2326,59 +2326,59 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="37" t="s">
         <v>167</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="37" t="s">
         <v>171</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="10"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="28"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C18" s="28"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="6"/>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="28"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="37"/>
       <c r="B19" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="C19" s="28"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="6"/>
       <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="28" t="s">
+      <c r="A20" s="37" t="s">
         <v>172</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="37" t="s">
         <v>175</v>
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="28"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="C21" s="28"/>
+      <c r="C21" s="37"/>
       <c r="D21" s="6"/>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>176</v>
       </c>
@@ -2402,7 +2402,7 @@
       <c r="D23" s="6"/>
       <c r="E23" s="9"/>
     </row>
-    <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="12" t="s">
         <v>181</v>
       </c>
@@ -2415,67 +2415,67 @@
       <c r="D24" s="6"/>
       <c r="E24" s="9"/>
     </row>
-    <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25" s="28" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="37" t="s">
         <v>184</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="C25" s="28"/>
+      <c r="C25" s="37"/>
       <c r="D25" s="6"/>
       <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="28"/>
+      <c r="A26" s="37"/>
       <c r="B26" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C26" s="28"/>
+      <c r="C26" s="37"/>
       <c r="D26" s="6"/>
       <c r="E26" s="9"/>
     </row>
-    <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27" s="28" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="37" t="s">
         <v>187</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="37" t="s">
         <v>190</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="9"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="28"/>
+      <c r="A28" s="37"/>
       <c r="B28" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="C28" s="28"/>
+      <c r="C28" s="37"/>
       <c r="D28" s="6"/>
       <c r="E28" s="9"/>
     </row>
-    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A29" s="28" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="37" t="s">
         <v>191</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="37" t="s">
         <v>194</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="9"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="28"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="12" t="s">
         <v>193</v>
       </c>
-      <c r="C30" s="28"/>
+      <c r="C30" s="37"/>
       <c r="D30" s="6"/>
       <c r="E30" s="9"/>
     </row>
@@ -2493,112 +2493,112 @@
       <c r="E31" s="9"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="37" t="s">
         <v>198</v>
       </c>
       <c r="B32" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="37" t="s">
         <v>201</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="28"/>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="37"/>
       <c r="B33" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="C33" s="28"/>
+      <c r="C33" s="37"/>
       <c r="D33" s="6"/>
       <c r="E33" s="9"/>
     </row>
-    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="28" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="37" t="s">
         <v>202</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="37" t="s">
         <v>205</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="9"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="28"/>
+      <c r="A35" s="37"/>
       <c r="B35" s="12" t="s">
         <v>204</v>
       </c>
-      <c r="C35" s="28"/>
+      <c r="C35" s="37"/>
       <c r="D35" s="6"/>
       <c r="E35" s="9"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="28" t="s">
+      <c r="A36" s="37" t="s">
         <v>206</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="37" t="s">
         <v>209</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="9"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="28"/>
+      <c r="A37" s="37"/>
       <c r="B37" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C37" s="28"/>
+      <c r="C37" s="37"/>
       <c r="D37" s="6"/>
       <c r="E37" s="9"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="28" t="s">
+      <c r="A38" s="37" t="s">
         <v>210</v>
       </c>
       <c r="B38" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="37" t="s">
         <v>213</v>
       </c>
       <c r="D38" s="6"/>
       <c r="E38" s="9"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="28"/>
+      <c r="A39" s="37"/>
       <c r="B39" s="12" t="s">
         <v>212</v>
       </c>
-      <c r="C39" s="28"/>
+      <c r="C39" s="37"/>
       <c r="D39" s="6"/>
       <c r="E39" s="9"/>
     </row>
-    <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="28" t="s">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="37" t="s">
         <v>214</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="37" t="s">
         <v>217</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="9"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="28"/>
+      <c r="A41" s="37"/>
       <c r="B41" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="C41" s="28"/>
+      <c r="C41" s="37"/>
       <c r="D41" s="6"/>
       <c r="E41" s="9"/>
     </row>
@@ -2612,6 +2612,18 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:C33"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="A34:A35"/>
@@ -2620,18 +2632,6 @@
     <mergeCell ref="C36:C37"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="C38:C39"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="C25:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2642,8 +2642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D0A090-A0FD-4C12-8A63-D35993E32FAB}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2944,7 +2944,7 @@
       <c r="E26" s="25">
         <v>2</v>
       </c>
-      <c r="F26" s="9"/>
+      <c r="F26" s="10"/>
     </row>
     <row r="27" spans="1:6" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
@@ -3146,7 +3146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0DC0284-78FD-4D6B-AB7A-95EC7E11330B}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -3159,19 +3159,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="33" t="s">
         <v>261</v>
       </c>
     </row>
@@ -3182,13 +3182,13 @@
       <c r="B2" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="30" t="s">
         <v>237</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="F2" s="35"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6" ht="29.4" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
@@ -3197,13 +3197,13 @@
       <c r="B3" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="30" t="s">
         <v>239</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>240</v>
       </c>
-      <c r="F3" s="35"/>
+      <c r="F3" s="34"/>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
@@ -3212,7 +3212,7 @@
       <c r="B4" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>241</v>
       </c>
       <c r="E4" s="12" t="s">
@@ -3229,13 +3229,13 @@
       <c r="B5" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>243</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="34"/>
     </row>
     <row r="6" spans="1:6" ht="29.4" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
@@ -3244,13 +3244,13 @@
       <c r="B6" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="30" t="s">
         <v>245</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:6" ht="29.4" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
@@ -3259,13 +3259,13 @@
       <c r="B7" s="12" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="31" t="s">
+      <c r="D7" s="30" t="s">
         <v>247</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="F7" s="35"/>
+      <c r="F7" s="34"/>
     </row>
     <row r="8" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
@@ -3274,13 +3274,13 @@
       <c r="B8" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="D8" s="31" t="s">
+      <c r="D8" s="30" t="s">
         <v>249</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="F8" s="35"/>
+      <c r="F8" s="34"/>
     </row>
     <row r="9" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
@@ -3289,49 +3289,49 @@
       <c r="B9" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>251</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="35"/>
     </row>
     <row r="10" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="30" t="s">
         <v>253</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>254</v>
       </c>
-      <c r="F10" s="37"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="31" t="s">
         <v>255</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="32" t="s">
         <v>256</v>
       </c>
-      <c r="F11" s="37"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="31" t="s">
         <v>257</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="32" t="s">
         <v>258</v>
       </c>
-      <c r="F12" s="37"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="31" t="s">
         <v>259</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="F13" s="37"/>
+      <c r="F13" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>